<commit_message>
updated passive rotations (different results here!)
</commit_message>
<xml_diff>
--- a/Passive_rotations/passive rotations results/degrees_of_liberty.xlsx
+++ b/Passive_rotations/passive rotations results/degrees_of_liberty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="135">
   <si>
     <t>Athlete</t>
   </si>
@@ -52,6 +52,18 @@
     <t>debut bras droit en haut, gauche bas,</t>
   </si>
   <si>
+    <t>KaFu bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>debut bras gauche en haut, droit bas,</t>
+  </si>
+  <si>
+    <t>KaFu bras en  bas, jambes tilt</t>
+  </si>
+  <si>
+    <t>bras en bas,</t>
+  </si>
+  <si>
     <t>LaDe bras en haut</t>
   </si>
   <si>
@@ -67,6 +79,12 @@
     <t>LaDe bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>LaDe bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>LaDe bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>WeEm bras en haut</t>
   </si>
   <si>
@@ -82,6 +100,12 @@
     <t>WeEm bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>WeEm bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>WeEm bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>AuJo bras en haut</t>
   </si>
   <si>
@@ -97,6 +121,12 @@
     <t>AuJo bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>AuJo bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>AuJo bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>AlAd bras en haut</t>
   </si>
   <si>
@@ -112,6 +142,12 @@
     <t>AlAd bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>AlAd bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>AlAd bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>FeBl bras en haut</t>
   </si>
   <si>
@@ -127,6 +163,12 @@
     <t>FeBl bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>FeBl bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>FeBl bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>MaJa bras en haut</t>
   </si>
   <si>
@@ -142,6 +184,12 @@
     <t>MaJa bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>MaJa bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>MaJa bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>JeCh bras en haut</t>
   </si>
   <si>
@@ -157,6 +205,12 @@
     <t>JeCh bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>JeCh bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>JeCh bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>MaCu bras en haut</t>
   </si>
   <si>
@@ -172,6 +226,12 @@
     <t>MaCu bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>MaCu bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>MaCu bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>ElMe bras en haut</t>
   </si>
   <si>
@@ -187,6 +247,12 @@
     <t>ElMe bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>ElMe bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>ElMe bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>KaMi bras en haut</t>
   </si>
   <si>
@@ -202,6 +268,12 @@
     <t>KaMi bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>KaMi bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>KaMi bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>ZoTs bras en haut</t>
   </si>
   <si>
@@ -217,6 +289,12 @@
     <t>ZoTs bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>ZoTs bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>ZoTs bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>Benjamin bras en haut</t>
   </si>
   <si>
@@ -232,6 +310,12 @@
     <t>Benjamin bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>Benjamin bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>Benjamin bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>Sarah bras en haut</t>
   </si>
   <si>
@@ -247,6 +331,12 @@
     <t>Sarah bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>Sarah bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>Sarah bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>AdCh bras en haut</t>
   </si>
   <si>
@@ -262,6 +352,12 @@
     <t>AdCh bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>AdCh bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>AdCh bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>EvZl bras en haut</t>
   </si>
   <si>
@@ -277,6 +373,12 @@
     <t>EvZl bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>EvZl bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>EvZl bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>SoMe bras en haut</t>
   </si>
   <si>
@@ -292,6 +394,12 @@
     <t>SoMe bras gauche bas, droit descend</t>
   </si>
   <si>
+    <t>SoMe bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>SoMe bras en  bas, jambes tilt</t>
+  </si>
+  <si>
     <t>OlGa bras en haut</t>
   </si>
   <si>
@@ -305,6 +413,12 @@
   </si>
   <si>
     <t>OlGa bras gauche bas, droit descend</t>
+  </si>
+  <si>
+    <t>OlGa bras droit bas, gauche descend</t>
+  </si>
+  <si>
+    <t>OlGa bras en  bas, jambes tilt</t>
   </si>
 </sst>
 </file>
@@ -636,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -743,478 +857,490 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>0.9999999999999983</v>
+        <v>1.091440158107889</v>
       </c>
       <c r="D7">
-        <v>-2.44671868459712E-18</v>
+        <v>-0.01602110439959128</v>
       </c>
       <c r="E7">
-        <v>-4.57759694566641E-17</v>
+        <v>-1.471486038173434</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>1.217855549853637</v>
+        <v>1.004441016787396</v>
       </c>
       <c r="D8">
-        <v>-4.190393164474243E-18</v>
+        <v>-0.01754656736373842</v>
       </c>
       <c r="E8">
-        <v>-7.064893470867802E-17</v>
+        <v>-0.3198313045813977</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>1.069160278824289</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D9">
-        <v>-0.02210695189542371</v>
+        <v>-2.44671868459712E-18</v>
       </c>
       <c r="E9">
-        <v>-1.428288876293047</v>
+        <v>-4.57759694566641E-17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10">
-        <v>1.094401980262778</v>
+        <v>1.217855549853637</v>
+      </c>
+      <c r="D10">
+        <v>-4.190393164474243E-18</v>
+      </c>
+      <c r="E10">
+        <v>-7.064893470867802E-17</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>1.08085630260126</v>
+        <v>1.069160278824289</v>
       </c>
       <c r="D11">
-        <v>0.01826611045667231</v>
+        <v>-0.02210695189542371</v>
       </c>
       <c r="E11">
-        <v>1.303046356021884</v>
+        <v>-1.428288876293047</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>0.9999999999999983</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+        <v>1.094401980262778</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>1.274435168921227</v>
+        <v>1.08085630260126</v>
       </c>
       <c r="D13">
-        <v>7.021436315136375E-19</v>
+        <v>0.01826611045667231</v>
       </c>
       <c r="E13">
-        <v>-3.607690238799585E-18</v>
+        <v>1.303046356021884</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1.080201400435422</v>
+        <v>1.08085630260126</v>
       </c>
       <c r="D14">
-        <v>-0.02811360159685304</v>
+        <v>-0.0182661104566723</v>
       </c>
       <c r="E14">
-        <v>-1.679621324394826</v>
+        <v>-1.303046356021884</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>1.114202317292074</v>
+        <v>1.003419214989376</v>
+      </c>
+      <c r="D15">
+        <v>-0.01867550072051027</v>
+      </c>
+      <c r="E15">
+        <v>-0.3222101441570804</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>1.107178622857474</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D16">
-        <v>0.02063787576870431</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1.489754181060191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0.9999999999999983</v>
+        <v>1.274435168921227</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>7.021436315136375E-19</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>-3.607690238799585E-18</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18">
-        <v>1.253494291100971</v>
+        <v>1.080201400435422</v>
       </c>
       <c r="D18">
-        <v>-6.158967387040388E-18</v>
+        <v>-0.02811360159685304</v>
       </c>
       <c r="E18">
-        <v>-7.118386281792429E-17</v>
+        <v>-1.679621324394826</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>1.083769045751328</v>
-      </c>
-      <c r="D19">
-        <v>-0.01646888777820121</v>
-      </c>
-      <c r="E19">
-        <v>-2.006741742533984</v>
+        <v>1.114202317292074</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>1.10705592940078</v>
+        <v>1.107178622857474</v>
+      </c>
+      <c r="D20">
+        <v>0.02063787576870431</v>
+      </c>
+      <c r="E20">
+        <v>1.489754181060191</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21">
-        <v>1.102152669145464</v>
+        <v>1.107178622857474</v>
       </c>
       <c r="D21">
-        <v>0.02072693612035587</v>
+        <v>-0.02063787576870432</v>
       </c>
       <c r="E21">
-        <v>1.809412728251673</v>
+        <v>-1.48975418106019</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>0.9999999999999983</v>
+        <v>0.9951791207551426</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>-0.02222176980644214</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-0.368102895682753</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23">
-        <v>1.287055527532938</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D23">
-        <v>-2.417713720151008E-19</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>1.344156931759271E-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
-        <v>1.098285484033857</v>
+        <v>1.253494291100971</v>
       </c>
       <c r="D24">
-        <v>-0.02711839299635802</v>
+        <v>-6.158967387040388E-18</v>
       </c>
       <c r="E24">
-        <v>-2.323862246878562</v>
+        <v>-7.118386281792429E-17</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25">
-        <v>1.118650249729702</v>
+        <v>1.083769045751328</v>
+      </c>
+      <c r="D25">
+        <v>-0.01646888777820121</v>
+      </c>
+      <c r="E25">
+        <v>-2.006741742533984</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>1.120372866450966</v>
-      </c>
-      <c r="D26">
-        <v>0.0219503448970936</v>
-      </c>
-      <c r="E26">
-        <v>2.057974428804151</v>
+        <v>1.10705592940078</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>0.9999999999999983</v>
+        <v>1.102152669145464</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.02072693612035587</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1.809412728251673</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>1.277441342429636</v>
+        <v>1.102152669145465</v>
       </c>
       <c r="D28">
-        <v>4.558793278028508E-18</v>
+        <v>-0.02072693612035565</v>
       </c>
       <c r="E28">
-        <v>6.552503540367981E-17</v>
+        <v>-1.809412728251671</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>1.090292460183105</v>
+        <v>1.002190607387618</v>
       </c>
       <c r="D29">
-        <v>-0.01707269966228063</v>
+        <v>-0.01900167409547302</v>
       </c>
       <c r="E29">
-        <v>-2.000689361272976</v>
+        <v>-0.3504079795833752</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="C30">
-        <v>1.115165486227972</v>
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>1.113346585979707</v>
+        <v>1.287055527532938</v>
       </c>
       <c r="D31">
-        <v>0.02219047356168109</v>
+        <v>-2.417713720151008E-19</v>
       </c>
       <c r="E31">
-        <v>1.789167367770335</v>
+        <v>1.344156931759271E-17</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32">
-        <v>0.9999999999999983</v>
+        <v>1.098285484033857</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>-0.02711839299635802</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>-2.323862246878562</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
-        <v>1.292532209241679</v>
-      </c>
-      <c r="D33">
-        <v>-2.762199754917321E-19</v>
-      </c>
-      <c r="E33">
-        <v>1.21437916361999E-17</v>
+        <v>1.118650249729702</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>1.101523626374624</v>
+        <v>1.120372866450966</v>
       </c>
       <c r="D34">
-        <v>-0.02184973511390472</v>
+        <v>0.0219503448970936</v>
       </c>
       <c r="E34">
-        <v>-2.200896638350306</v>
+        <v>2.057974428804151</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C35">
-        <v>1.120841297614019</v>
+        <v>1.120372866450966</v>
+      </c>
+      <c r="D35">
+        <v>-0.02195034489709373</v>
+      </c>
+      <c r="E35">
+        <v>-2.057974428804152</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C36">
-        <v>1.121511342759407</v>
+        <v>0.9981497052735353</v>
       </c>
       <c r="D36">
-        <v>0.0199943348545901</v>
+        <v>-0.01930966060856861</v>
       </c>
       <c r="E36">
-        <v>1.963412743116275</v>
+        <v>-0.3824221836853463</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -1231,543 +1357,555 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38">
-        <v>1.339904385380295</v>
+        <v>1.277441342429636</v>
       </c>
       <c r="D38">
-        <v>-3.359153448221651E-18</v>
+        <v>4.558793278028508E-18</v>
       </c>
       <c r="E38">
-        <v>-2.385551302481234E-17</v>
+        <v>6.552503540367981E-17</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39">
-        <v>1.097542830153251</v>
+        <v>1.090292460183105</v>
       </c>
       <c r="D39">
-        <v>-0.03050151172285825</v>
+        <v>-0.01707269966228063</v>
       </c>
       <c r="E39">
-        <v>-1.688974724371944</v>
+        <v>-2.000689361272976</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40">
-        <v>1.137838463189823</v>
+        <v>1.115165486227972</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41">
-        <v>1.132047429720109</v>
+        <v>1.113346585979707</v>
       </c>
       <c r="D41">
-        <v>0.02332862796727719</v>
+        <v>0.02219047356168109</v>
       </c>
       <c r="E41">
-        <v>1.473234795998403</v>
+        <v>1.789167367770335</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>0.9999999999999983</v>
+        <v>1.113346585979707</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>-0.022190473561681</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>-1.789167367770335</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C43">
-        <v>1.233052296225167</v>
+        <v>0.998443728754405</v>
       </c>
       <c r="D43">
-        <v>1.088211766262488E-19</v>
+        <v>-0.01998914382559783</v>
       </c>
       <c r="E43">
-        <v>5.872824480692875E-19</v>
+        <v>-0.3709188150538064</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
       </c>
       <c r="C44">
-        <v>1.068565923450456</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D44">
-        <v>-0.02632300416324719</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>-1.637807772454535</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
       <c r="C45">
-        <v>1.09949940659226</v>
+        <v>1.292532209241679</v>
+      </c>
+      <c r="D45">
+        <v>-2.762199754917321E-19</v>
+      </c>
+      <c r="E45">
+        <v>1.21437916361999E-17</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>1.087304116680685</v>
+        <v>1.101523626374624</v>
       </c>
       <c r="D46">
-        <v>0.01849335363197831</v>
+        <v>-0.02184973511390472</v>
       </c>
       <c r="E46">
-        <v>1.476687605840129</v>
+        <v>-2.200896638350306</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
       <c r="C47">
-        <v>0.9999999999999983</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
+        <v>1.120841297614019</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>1.256882609233365</v>
+        <v>1.121511342759407</v>
       </c>
       <c r="D48">
-        <v>-6.313695791847065E-18</v>
+        <v>0.0199943348545901</v>
       </c>
       <c r="E48">
-        <v>-8.800136566741688E-17</v>
+        <v>1.963412743116275</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>1.086890448045416</v>
+        <v>1.121511342759408</v>
       </c>
       <c r="D49">
-        <v>-0.01624557550090589</v>
+        <v>-0.01999433485458999</v>
       </c>
       <c r="E49">
-        <v>-2.019342915642726</v>
+        <v>-1.963412743116276</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>1.108287388639786</v>
+        <v>0.9955643020329721</v>
+      </c>
+      <c r="D50">
+        <v>-0.02199924076772516</v>
+      </c>
+      <c r="E50">
+        <v>-0.414616035110914</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>1.105467739087892</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D51">
-        <v>0.02034417229317992</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>1.820940204468787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52">
-        <v>0.9999999999999983</v>
+        <v>1.339904385380295</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>-3.359153448221651E-18</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>-2.385551302481234E-17</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
       </c>
       <c r="C53">
-        <v>1.261548804027901</v>
+        <v>1.097542830153251</v>
       </c>
       <c r="D53">
-        <v>4.165542200342571E-19</v>
+        <v>-0.03050151172285825</v>
       </c>
       <c r="E53">
-        <v>5.195882885681811E-18</v>
+        <v>-1.688974724371944</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
       </c>
       <c r="C54">
-        <v>1.082641483337514</v>
-      </c>
-      <c r="D54">
-        <v>-0.01721422038893254</v>
-      </c>
-      <c r="E54">
-        <v>-1.877446215873254</v>
+        <v>1.137838463189823</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C55">
-        <v>1.110601893208074</v>
+        <v>1.132047429720109</v>
+      </c>
+      <c r="D55">
+        <v>0.02332862796727719</v>
+      </c>
+      <c r="E55">
+        <v>1.473234795998403</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C56">
-        <v>1.106965825634767</v>
+        <v>1.132047429720109</v>
       </c>
       <c r="D56">
-        <v>0.01951227300687495</v>
+        <v>-0.02332862796727751</v>
       </c>
       <c r="E56">
-        <v>1.684499501227019</v>
+        <v>-1.473234795998404</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C57">
-        <v>0.9999999999999983</v>
+        <v>0.9887896416466514</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>-0.02477650052620019</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>-0.3879688375396535</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
       <c r="C58">
-        <v>1.233063899435188</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D58">
-        <v>-1.100656534464553E-19</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>7.342169756745331E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
       </c>
       <c r="C59">
-        <v>1.076639092418431</v>
+        <v>1.233052296225167</v>
       </c>
       <c r="D59">
-        <v>-0.02324000745072328</v>
+        <v>1.088211766262488E-19</v>
       </c>
       <c r="E59">
-        <v>-1.441453243690183</v>
+        <v>5.872824480692875E-19</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
       <c r="C60">
-        <v>1.100320792972959</v>
+        <v>1.068565923450456</v>
+      </c>
+      <c r="D60">
+        <v>-0.02632300416324719</v>
+      </c>
+      <c r="E60">
+        <v>-1.637807772454535</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>1.089935456096748</v>
-      </c>
-      <c r="D61">
-        <v>0.01914098728762189</v>
-      </c>
-      <c r="E61">
-        <v>1.312553932270934</v>
+        <v>1.09949940659226</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C62">
-        <v>0.9999999999999983</v>
+        <v>1.087304116680685</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>0.01849335363197831</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1.476687605840129</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C63">
-        <v>1.25260105879694</v>
+        <v>1.087304116680685</v>
       </c>
       <c r="D63">
-        <v>-8.351015275557645E-19</v>
+        <v>-0.01849335363197844</v>
       </c>
       <c r="E63">
-        <v>-1.946209277132925E-18</v>
+        <v>-1.476687605840131</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C64">
-        <v>1.078714914409214</v>
+        <v>0.997582159317207</v>
       </c>
       <c r="D64">
-        <v>-0.0162592795501383</v>
+        <v>-0.02069059124756667</v>
       </c>
       <c r="E64">
-        <v>-1.931888789898742</v>
+        <v>-0.358369295041212</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
       </c>
       <c r="C65">
-        <v>1.106738191019348</v>
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C66">
-        <v>1.101164070273127</v>
+        <v>1.256882609233365</v>
       </c>
       <c r="D66">
-        <v>0.02011393460000948</v>
+        <v>-6.313695791847065E-18</v>
       </c>
       <c r="E66">
-        <v>1.711955996533278</v>
+        <v>-8.800136566741688E-17</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
       <c r="C67">
-        <v>0.9999999999999983</v>
+        <v>1.086890448045416</v>
       </c>
       <c r="D67">
-        <v>-1.434986353764051E-19</v>
+        <v>-0.01624557550090589</v>
       </c>
       <c r="E67">
-        <v>2.941354821778473E-20</v>
+        <v>-2.019342915642726</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
       </c>
       <c r="C68">
-        <v>1.398724353571791</v>
-      </c>
-      <c r="D68">
-        <v>2.203620500293367E-17</v>
-      </c>
-      <c r="E68">
-        <v>2.226485961086121E-16</v>
+        <v>1.108287388639786</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C69">
-        <v>1.124016184227355</v>
+        <v>1.105467739087892</v>
       </c>
       <c r="D69">
-        <v>-0.02108673807532865</v>
+        <v>0.02034417229317992</v>
       </c>
       <c r="E69">
-        <v>-1.803890593774745</v>
+        <v>1.820940204468787</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C70">
-        <v>1.158804495250084</v>
+        <v>1.105467739087892</v>
+      </c>
+      <c r="D70">
+        <v>-0.02034417229318007</v>
+      </c>
+      <c r="E70">
+        <v>-1.820940204468788</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C71">
-        <v>1.167904961393588</v>
+        <v>1.002833708019202</v>
       </c>
       <c r="D71">
-        <v>0.02147478262540211</v>
+        <v>-0.01892131098947303</v>
       </c>
       <c r="E71">
-        <v>1.586242423538427</v>
+        <v>-0.3551611729253452</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -1784,301 +1922,889 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
       </c>
       <c r="C73">
-        <v>1.342953182027163</v>
+        <v>1.261548804027901</v>
       </c>
       <c r="D73">
-        <v>-9.385736727878577E-19</v>
+        <v>4.165542200342571E-19</v>
       </c>
       <c r="E73">
-        <v>-6.809850679750789E-18</v>
+        <v>5.195882885681811E-18</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="C74">
-        <v>1.115239515852464</v>
+        <v>1.082641483337514</v>
       </c>
       <c r="D74">
-        <v>-0.02957999657747152</v>
+        <v>-0.01721422038893254</v>
       </c>
       <c r="E74">
-        <v>-2.268351886391657</v>
+        <v>-1.877446215873254</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
       </c>
       <c r="C75">
-        <v>1.137464995268932</v>
+        <v>1.110601893208074</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
       </c>
       <c r="C76">
-        <v>1.143105065399169</v>
+        <v>1.106965825634767</v>
       </c>
       <c r="D76">
-        <v>0.02559901748360066</v>
+        <v>0.01951227300687495</v>
       </c>
       <c r="E76">
-        <v>1.980242608179293</v>
+        <v>1.684499501227019</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>0.9999999999999983</v>
+        <v>1.106965825634767</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>-0.01951227300687506</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>-1.68449950122702</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C78">
-        <v>1.257688840511566</v>
+        <v>1.001593336430482</v>
       </c>
       <c r="D78">
-        <v>-8.205821791222056E-20</v>
+        <v>-0.01907960091631204</v>
       </c>
       <c r="E78">
-        <v>-7.01125993311276E-18</v>
+        <v>-0.3557038426710678</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
       </c>
       <c r="C79">
-        <v>1.091182937779898</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D79">
-        <v>-0.01671795355797989</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>-2.112491541888866</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
       </c>
       <c r="C80">
-        <v>1.109099065797873</v>
+        <v>1.233063899435188</v>
+      </c>
+      <c r="D80">
+        <v>-1.100656534464553E-19</v>
+      </c>
+      <c r="E80">
+        <v>7.342169756745331E-19</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C81">
-        <v>1.10624435453879</v>
+        <v>1.076639092418431</v>
       </c>
       <c r="D81">
-        <v>0.01789717113135894</v>
+        <v>-0.02324000745072328</v>
       </c>
       <c r="E81">
-        <v>1.910167930087624</v>
+        <v>-1.441453243690183</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82">
-        <v>0.9999999999999983</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
+        <v>1.100320792972959</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C83">
-        <v>1.213487695493514</v>
+        <v>1.089935456096748</v>
       </c>
       <c r="D83">
-        <v>-1.782188905793229E-18</v>
+        <v>0.01914098728762189</v>
       </c>
       <c r="E83">
-        <v>-1.641014805782282E-17</v>
+        <v>1.312553932270934</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C84">
-        <v>1.066558320064056</v>
+        <v>1.089935456096748</v>
       </c>
       <c r="D84">
-        <v>-0.02355826215774664</v>
+        <v>-0.01914098728762172</v>
       </c>
       <c r="E84">
-        <v>-1.401830081035538</v>
+        <v>-1.312553932270935</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C85">
-        <v>1.092639845174732</v>
+        <v>1.007453064085008</v>
+      </c>
+      <c r="D85">
+        <v>-0.01533584660896769</v>
+      </c>
+      <c r="E85">
+        <v>-0.2776168427697701</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C86">
-        <v>1.077884014343934</v>
+        <v>0.9999999999999983</v>
       </c>
       <c r="D86">
-        <v>0.01957244601449594</v>
+        <v>0</v>
       </c>
       <c r="E86">
-        <v>1.272440181192728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
       </c>
       <c r="C87">
-        <v>0.9999999999999983</v>
+        <v>1.25260105879694</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>-8.351015275557645E-19</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>-1.946209277132925E-18</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
       </c>
       <c r="C88">
-        <v>1.271955500213589</v>
+        <v>1.078714914409214</v>
       </c>
       <c r="D88">
-        <v>3.472728191951902E-19</v>
+        <v>-0.0162592795501383</v>
       </c>
       <c r="E88">
-        <v>-2.021641664657118E-18</v>
+        <v>-1.931888789898742</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
       </c>
       <c r="C89">
-        <v>1.084160439248087</v>
-      </c>
-      <c r="D89">
-        <v>-0.0179155055440622</v>
-      </c>
-      <c r="E89">
-        <v>-1.947413087836881</v>
+        <v>1.106738191019348</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C90">
-        <v>1.113692625131941</v>
+        <v>1.101164070273127</v>
+      </c>
+      <c r="D90">
+        <v>0.02011393460000948</v>
+      </c>
+      <c r="E90">
+        <v>1.711955996533278</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91">
+        <v>1.101164070273127</v>
+      </c>
+      <c r="D91">
+        <v>-0.02011393460000933</v>
+      </c>
+      <c r="E91">
+        <v>-1.711955996533277</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92">
+        <v>0.9953570640860281</v>
+      </c>
+      <c r="D92">
+        <v>-0.01930560940248675</v>
+      </c>
+      <c r="E92">
+        <v>-0.3913513232841628</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D93">
+        <v>-1.434986353764051E-19</v>
+      </c>
+      <c r="E93">
+        <v>2.941354821778473E-20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>1.398724353571791</v>
+      </c>
+      <c r="D94">
+        <v>2.203620500293367E-17</v>
+      </c>
+      <c r="E94">
+        <v>2.226485961086121E-16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95">
+        <v>1.124016184227355</v>
+      </c>
+      <c r="D95">
+        <v>-0.02108673807532865</v>
+      </c>
+      <c r="E95">
+        <v>-1.803890593774745</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>1.158804495250084</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>104</v>
+      </c>
+      <c r="B97" t="s">
         <v>11</v>
       </c>
-      <c r="C91">
+      <c r="C97">
+        <v>1.167904961393588</v>
+      </c>
+      <c r="D97">
+        <v>0.02147478262540211</v>
+      </c>
+      <c r="E97">
+        <v>1.586242423538427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>105</v>
+      </c>
+      <c r="B98" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98">
+        <v>1.167904961393588</v>
+      </c>
+      <c r="D98">
+        <v>-0.02147478262540212</v>
+      </c>
+      <c r="E98">
+        <v>-1.586242423538427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99">
+        <v>0.9958230384706586</v>
+      </c>
+      <c r="D99">
+        <v>-0.02456898470107204</v>
+      </c>
+      <c r="E99">
+        <v>-0.3778440894182061</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>108</v>
+      </c>
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101">
+        <v>1.342953182027163</v>
+      </c>
+      <c r="D101">
+        <v>-9.385736727878577E-19</v>
+      </c>
+      <c r="E101">
+        <v>-6.809850679750789E-18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>109</v>
+      </c>
+      <c r="B102" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102">
+        <v>1.115239515852464</v>
+      </c>
+      <c r="D102">
+        <v>-0.02957999657747152</v>
+      </c>
+      <c r="E102">
+        <v>-2.268351886391657</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103">
+        <v>1.137464995268932</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104">
+        <v>1.143105065399169</v>
+      </c>
+      <c r="D104">
+        <v>0.02559901748360066</v>
+      </c>
+      <c r="E104">
+        <v>1.980242608179293</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105">
+        <v>1.143105065399169</v>
+      </c>
+      <c r="D105">
+        <v>-0.02559901748360066</v>
+      </c>
+      <c r="E105">
+        <v>-1.980242608179295</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>113</v>
+      </c>
+      <c r="B106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106">
+        <v>0.9940969291593699</v>
+      </c>
+      <c r="D106">
+        <v>-0.02204014846240779</v>
+      </c>
+      <c r="E106">
+        <v>-0.3901238839456873</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107">
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>1.257688840511566</v>
+      </c>
+      <c r="D108">
+        <v>-8.205821791222056E-20</v>
+      </c>
+      <c r="E108">
+        <v>-7.01125993311276E-18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>1.091182937779898</v>
+      </c>
+      <c r="D109">
+        <v>-0.01671795355797989</v>
+      </c>
+      <c r="E109">
+        <v>-2.112491541888866</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>117</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110">
+        <v>1.109099065797873</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111">
+        <v>1.10624435453879</v>
+      </c>
+      <c r="D111">
+        <v>0.01789717113135894</v>
+      </c>
+      <c r="E111">
+        <v>1.910167930087624</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112">
+        <v>1.106244354538791</v>
+      </c>
+      <c r="D112">
+        <v>-0.01789717113135892</v>
+      </c>
+      <c r="E112">
+        <v>-1.910167930087628</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113">
+        <v>1.000593129380023</v>
+      </c>
+      <c r="D113">
+        <v>-0.01902920884972461</v>
+      </c>
+      <c r="E113">
+        <v>-0.3848441196364908</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>121</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114">
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>122</v>
+      </c>
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115">
+        <v>1.213487695493514</v>
+      </c>
+      <c r="D115">
+        <v>-1.782188905793229E-18</v>
+      </c>
+      <c r="E115">
+        <v>-1.641014805782282E-17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>123</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116">
+        <v>1.066558320064056</v>
+      </c>
+      <c r="D116">
+        <v>-0.02355826215774664</v>
+      </c>
+      <c r="E116">
+        <v>-1.401830081035538</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>124</v>
+      </c>
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117">
+        <v>1.092639845174732</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>125</v>
+      </c>
+      <c r="B118" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118">
+        <v>1.077884014343934</v>
+      </c>
+      <c r="D118">
+        <v>0.01957244601449594</v>
+      </c>
+      <c r="E118">
+        <v>1.272440181192728</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>126</v>
+      </c>
+      <c r="B119" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119">
+        <v>1.077884014343934</v>
+      </c>
+      <c r="D119">
+        <v>-0.01957244601449596</v>
+      </c>
+      <c r="E119">
+        <v>-1.272440181192728</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>127</v>
+      </c>
+      <c r="B120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120">
+        <v>0.999961608477812</v>
+      </c>
+      <c r="D120">
+        <v>-0.02034535629583191</v>
+      </c>
+      <c r="E120">
+        <v>-0.341879944381002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>128</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121">
+        <v>0.9999999999999983</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>129</v>
+      </c>
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122">
+        <v>1.271955500213589</v>
+      </c>
+      <c r="D122">
+        <v>3.472728191951902E-19</v>
+      </c>
+      <c r="E122">
+        <v>-2.021641664657118E-18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>130</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <v>1.084160439248087</v>
+      </c>
+      <c r="D123">
+        <v>-0.0179155055440622</v>
+      </c>
+      <c r="E123">
+        <v>-1.947413087836881</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>131</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>1.113692625131941</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>132</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125">
         <v>1.108470098782997</v>
       </c>
-      <c r="D91">
+      <c r="D125">
         <v>0.02289783772729734</v>
       </c>
-      <c r="E91">
+      <c r="E125">
         <v>1.729815865321129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>133</v>
+      </c>
+      <c r="B126" t="s">
+        <v>13</v>
+      </c>
+      <c r="C126">
+        <v>1.108470098782995</v>
+      </c>
+      <c r="D126">
+        <v>-0.02289783772729731</v>
+      </c>
+      <c r="E126">
+        <v>-1.72981586532113</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>134</v>
+      </c>
+      <c r="B127" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127">
+        <v>0.9966486739826913</v>
+      </c>
+      <c r="D127">
+        <v>-0.0210498612691505</v>
+      </c>
+      <c r="E127">
+        <v>-0.3758066160436499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>